<commit_message>
updated genotyping analysis based on MAFFT parallelism fix.
</commit_message>
<xml_diff>
--- a/tabular/genotypingAnalysis.xlsx
+++ b/tabular/genotypingAnalysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="1420" windowWidth="47320" windowHeight="19000" tabRatio="500"/>
+    <workbookView xWindow="7180" yWindow="2960" windowWidth="47320" windowHeight="19000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Neither metadata, EPA nor ViPR define genotype</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>finalCladeCutoff</t>
+  </si>
+  <si>
+    <t>Fixed MAFFT parallelism</t>
   </si>
 </sst>
 </file>
@@ -314,8 +317,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,7 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -434,6 +441,8 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -467,6 +476,8 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -800,117 +811,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="50.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>82928</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="D3" s="2">
+        <v>82928</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>1779</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="D4" s="2">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:15">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:16" s="14" customFormat="1">
+    <row r="8" spans="1:15" s="14" customFormat="1">
       <c r="A8" s="14" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="14">
         <v>-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" s="14" customFormat="1">
+      <c r="D8" s="14">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="14" customFormat="1">
       <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="14">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" s="14" customFormat="1">
+      <c r="D9" s="14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="14" customFormat="1">
       <c r="A10" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="14">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" s="4" customFormat="1">
+      <c r="D10" s="14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="4" customFormat="1">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:16" s="4" customFormat="1">
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" s="4" customFormat="1">
       <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="4">
         <v>58775</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="D13" s="4">
+        <v>60458</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="4" customFormat="1">
+    <row r="14" spans="1:15" s="4" customFormat="1">
       <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="4">
         <v>477</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" s="4" customFormat="1">
+      <c r="D14" s="4">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="4" customFormat="1">
       <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="4">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" s="4" customFormat="1">
+      <c r="D15" s="4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="4" customFormat="1">
       <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>44</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="4" customFormat="1">
@@ -920,6 +963,9 @@
       <c r="B17" s="4">
         <v>2</v>
       </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1">
       <c r="A18" s="6" t="s">
@@ -927,6 +973,9 @@
       </c>
       <c r="B18" s="4">
         <v>59325</v>
+      </c>
+      <c r="D18" s="4">
+        <v>61049</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="8" customFormat="1">
@@ -941,6 +990,9 @@
       <c r="B20" s="8">
         <v>4944</v>
       </c>
+      <c r="D20" s="8">
+        <v>5013</v>
+      </c>
     </row>
     <row r="21" spans="1:4" s="8" customFormat="1">
       <c r="A21" s="9" t="s">
@@ -949,8 +1001,11 @@
       <c r="B21" s="8">
         <v>26</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>45</v>
+      </c>
+      <c r="D21" s="8">
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="8" customFormat="1">
@@ -959,6 +1014,9 @@
       </c>
       <c r="B22" s="8">
         <v>4970</v>
+      </c>
+      <c r="D22" s="8">
+        <v>5039</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="4" customFormat="1">
@@ -973,6 +1031,9 @@
       <c r="B24" s="4">
         <v>1695</v>
       </c>
+      <c r="D24" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1">
       <c r="A25" s="6" t="s">
@@ -981,6 +1042,9 @@
       <c r="B25" s="4">
         <v>48</v>
       </c>
+      <c r="D25" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:4" s="4" customFormat="1">
       <c r="A26" s="6" t="s">
@@ -989,8 +1053,11 @@
       <c r="B26" s="4">
         <v>1743</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>47</v>
+      </c>
+      <c r="D26" s="4">
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="8" customFormat="1">
@@ -1005,8 +1072,11 @@
       <c r="B28" s="8">
         <v>100</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>45</v>
+      </c>
+      <c r="D28" s="8">
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="4" customFormat="1">
@@ -1021,6 +1091,9 @@
       <c r="B30" s="4">
         <v>13803</v>
       </c>
+      <c r="D30" s="4">
+        <v>13977</v>
+      </c>
     </row>
     <row r="31" spans="1:4" s="4" customFormat="1">
       <c r="A31" s="6" t="s">
@@ -1029,6 +1102,9 @@
       <c r="B31" s="4">
         <v>982</v>
       </c>
+      <c r="D31" s="4">
+        <v>986</v>
+      </c>
     </row>
     <row r="32" spans="1:4" s="4" customFormat="1">
       <c r="A32" s="6" t="s">
@@ -1036,6 +1112,9 @@
       </c>
       <c r="B32" s="4">
         <v>14785</v>
+      </c>
+      <c r="D32" s="4">
+        <v>14963</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="8" customFormat="1">
@@ -1050,6 +1129,9 @@
       <c r="B34" s="8">
         <v>1791</v>
       </c>
+      <c r="D34" s="8">
+        <v>1792</v>
+      </c>
     </row>
     <row r="35" spans="1:4" s="4" customFormat="1">
       <c r="A35" s="3" t="s">
@@ -1063,8 +1145,11 @@
       <c r="B36" s="4">
         <v>182</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>47</v>
+      </c>
+      <c r="D36" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="8" customFormat="1">
@@ -1079,6 +1164,9 @@
       <c r="B38" s="8">
         <v>32</v>
       </c>
+      <c r="D38" s="8">
+        <v>31</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
@@ -1095,6 +1183,9 @@
       <c r="B43" s="14">
         <v>-3</v>
       </c>
+      <c r="D43" s="14">
+        <v>-3</v>
+      </c>
     </row>
     <row r="44" spans="1:4" s="14" customFormat="1">
       <c r="A44" s="14" t="s">
@@ -1103,6 +1194,9 @@
       <c r="B44" s="14">
         <v>0.26</v>
       </c>
+      <c r="D44" s="14">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="45" spans="1:4" s="14" customFormat="1">
       <c r="A45" s="14" t="s">
@@ -1111,6 +1205,9 @@
       <c r="B45" s="14">
         <v>80</v>
       </c>
+      <c r="D45" s="14">
+        <v>80</v>
+      </c>
     </row>
     <row r="47" spans="1:4" s="11" customFormat="1">
       <c r="A47" s="10" t="s">
@@ -1124,8 +1221,11 @@
       <c r="B48" s="11">
         <v>54017</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="C48" s="11" t="s">
         <v>48</v>
+      </c>
+      <c r="D48" s="11">
+        <v>55490</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="11" customFormat="1">
@@ -1135,6 +1235,9 @@
       <c r="B49" s="11">
         <v>1348</v>
       </c>
+      <c r="D49" s="11">
+        <v>1388</v>
+      </c>
     </row>
     <row r="50" spans="1:4" s="11" customFormat="1">
       <c r="A50" s="11" t="s">
@@ -1143,6 +1246,9 @@
       <c r="B50" s="11">
         <v>1077</v>
       </c>
+      <c r="D50" s="11">
+        <v>1079</v>
+      </c>
     </row>
     <row r="51" spans="1:4" s="11" customFormat="1">
       <c r="A51" s="11" t="s">
@@ -1151,8 +1257,11 @@
       <c r="B51" s="11">
         <v>47</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="C51" s="11" t="s">
         <v>51</v>
+      </c>
+      <c r="D51" s="11">
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="11" customFormat="1">
@@ -1162,8 +1271,11 @@
       <c r="B52" s="11">
         <v>4</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="C52" s="11" t="s">
         <v>46</v>
+      </c>
+      <c r="D52" s="11">
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="11" customFormat="1">
@@ -1172,6 +1284,9 @@
       </c>
       <c r="B53" s="11">
         <v>56493</v>
+      </c>
+      <c r="D53" s="11">
+        <v>58008</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="13" customFormat="1">
@@ -1186,8 +1301,11 @@
       <c r="B55" s="13">
         <v>4443</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="C55" s="13" t="s">
         <v>48</v>
+      </c>
+      <c r="D55" s="13">
+        <v>4506</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="13" customFormat="1">
@@ -1197,6 +1315,9 @@
       <c r="B56" s="13">
         <v>206</v>
       </c>
+      <c r="D56" s="13">
+        <v>206</v>
+      </c>
     </row>
     <row r="57" spans="1:4" s="13" customFormat="1">
       <c r="A57" s="13" t="s">
@@ -1204,6 +1325,9 @@
       </c>
       <c r="B57" s="13">
         <v>4649</v>
+      </c>
+      <c r="D57" s="13">
+        <v>4712</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="11" customFormat="1">
@@ -1218,6 +1342,9 @@
       <c r="B59" s="11">
         <v>1485</v>
       </c>
+      <c r="D59" s="11">
+        <v>12</v>
+      </c>
     </row>
     <row r="60" spans="1:4" s="11" customFormat="1">
       <c r="A60" s="11" t="s">
@@ -1226,6 +1353,9 @@
       <c r="B60" s="11">
         <v>56</v>
       </c>
+      <c r="D60" s="11">
+        <v>14</v>
+      </c>
     </row>
     <row r="61" spans="1:4" s="11" customFormat="1">
       <c r="A61" s="11" t="s">
@@ -1234,8 +1364,11 @@
       <c r="B61" s="11">
         <v>1541</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="C61" s="11" t="s">
         <v>47</v>
+      </c>
+      <c r="D61" s="11">
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="13" customFormat="1">
@@ -1250,8 +1383,11 @@
       <c r="B63" s="13">
         <v>194</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="C63" s="8" t="s">
         <v>45</v>
+      </c>
+      <c r="D63" s="13">
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="11" customFormat="1">
@@ -1266,8 +1402,11 @@
       <c r="B65" s="11">
         <v>16095</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="C65" s="11" t="s">
         <v>48</v>
+      </c>
+      <c r="D65" s="11">
+        <v>16676</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="11" customFormat="1">
@@ -1277,6 +1416,9 @@
       <c r="B66" s="11">
         <v>1281</v>
       </c>
+      <c r="D66" s="11">
+        <v>1306</v>
+      </c>
     </row>
     <row r="67" spans="1:4" s="11" customFormat="1">
       <c r="A67" s="11" t="s">
@@ -1284,6 +1426,9 @@
       </c>
       <c r="B67" s="11">
         <v>17376</v>
+      </c>
+      <c r="D67" s="11">
+        <v>17982</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="13" customFormat="1">
@@ -1298,6 +1443,9 @@
       <c r="B69" s="13">
         <v>1662</v>
       </c>
+      <c r="D69" s="13">
+        <v>1664</v>
+      </c>
     </row>
     <row r="70" spans="1:4" s="11" customFormat="1">
       <c r="A70" s="10" t="s">
@@ -1311,6 +1459,9 @@
       <c r="B71" s="11">
         <v>625</v>
       </c>
+      <c r="D71" s="11">
+        <v>19</v>
+      </c>
     </row>
     <row r="72" spans="1:4" s="13" customFormat="1">
       <c r="A72" s="12" t="s">
@@ -1323,6 +1474,9 @@
       </c>
       <c r="B73" s="13">
         <v>388</v>
+      </c>
+      <c r="D73" s="13">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incorporate updated genotypes and LANL metadata into the build.
</commit_message>
<xml_diff>
--- a/tabular/genotypingAnalysis.xlsx
+++ b/tabular/genotypingAnalysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="2960" windowWidth="47320" windowHeight="19000" tabRatio="500"/>
+    <workbookView xWindow="4100" yWindow="14480" windowWidth="44000" windowHeight="11640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Neither metadata, EPA nor ViPR define genotype</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Fixed MAFFT parallelism</t>
+  </si>
+  <si>
+    <t>Updated clade definitions</t>
   </si>
 </sst>
 </file>
@@ -317,7 +320,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -389,8 +392,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -406,8 +413,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -443,6 +451,8 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -478,6 +488,8 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -813,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -823,7 +835,8 @@
     <col min="2" max="2" width="18.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="22.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -836,6 +849,9 @@
       <c r="D1" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="E1" s="15" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
@@ -847,6 +863,9 @@
       <c r="D3" s="2">
         <v>82928</v>
       </c>
+      <c r="E3" s="2">
+        <v>82928</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
@@ -858,6 +877,9 @@
       <c r="D4" s="2">
         <v>1779</v>
       </c>
+      <c r="E4" s="2">
+        <v>1779</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
@@ -877,6 +899,9 @@
       <c r="D8" s="14">
         <v>-3</v>
       </c>
+      <c r="E8" s="14">
+        <v>-3</v>
+      </c>
     </row>
     <row r="9" spans="1:15" s="14" customFormat="1">
       <c r="A9" s="14" t="s">
@@ -888,6 +913,9 @@
       <c r="D9" s="14">
         <v>0.4</v>
       </c>
+      <c r="E9" s="14">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="10" spans="1:15" s="14" customFormat="1">
       <c r="A10" s="14" t="s">
@@ -899,6 +927,9 @@
       <c r="D10" s="14">
         <v>80</v>
       </c>
+      <c r="E10" s="14">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="1:15" s="4" customFormat="1">
       <c r="A12" s="3" t="s">
@@ -916,6 +947,9 @@
       <c r="D13" s="4">
         <v>60458</v>
       </c>
+      <c r="E13" s="4">
+        <v>60464</v>
+      </c>
       <c r="O13" s="4" t="s">
         <v>28</v>
       </c>
@@ -930,6 +964,9 @@
       <c r="D14" s="4">
         <v>518</v>
       </c>
+      <c r="E14" s="4">
+        <v>518</v>
+      </c>
     </row>
     <row r="15" spans="1:15" s="4" customFormat="1">
       <c r="A15" s="6" t="s">
@@ -941,6 +978,9 @@
       <c r="D15" s="4">
         <v>71</v>
       </c>
+      <c r="E15" s="4">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="1:15" s="4" customFormat="1">
       <c r="A16" s="6" t="s">
@@ -955,8 +995,11 @@
       <c r="D16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" s="4" customFormat="1">
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1">
       <c r="A17" s="6" t="s">
         <v>9</v>
       </c>
@@ -966,8 +1009,11 @@
       <c r="D17" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" s="4" customFormat="1">
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="4" customFormat="1">
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
@@ -977,13 +1023,16 @@
       <c r="D18" s="4">
         <v>61049</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" s="8" customFormat="1">
+      <c r="E18" s="4">
+        <v>61055</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="8" customFormat="1">
+    <row r="20" spans="1:5" s="8" customFormat="1">
       <c r="A20" s="9" t="s">
         <v>10</v>
       </c>
@@ -993,8 +1042,11 @@
       <c r="D20" s="8">
         <v>5013</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" s="8" customFormat="1">
+      <c r="E20" s="8">
+        <v>5019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="8" customFormat="1">
       <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
@@ -1007,8 +1059,11 @@
       <c r="D21" s="8">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" s="8" customFormat="1">
+      <c r="E21" s="8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="8" customFormat="1">
       <c r="A22" s="9" t="s">
         <v>4</v>
       </c>
@@ -1018,13 +1073,16 @@
       <c r="D22" s="8">
         <v>5039</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="4" customFormat="1">
+      <c r="E22" s="8">
+        <v>5045</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="4" customFormat="1">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="4" customFormat="1">
+    <row r="24" spans="1:5" s="4" customFormat="1">
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
@@ -1034,8 +1092,11 @@
       <c r="D24" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" s="4" customFormat="1">
+      <c r="E24" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="4" customFormat="1">
       <c r="A25" s="6" t="s">
         <v>13</v>
       </c>
@@ -1045,8 +1106,11 @@
       <c r="D25" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" s="4" customFormat="1">
+      <c r="E25" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="4" customFormat="1">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
@@ -1059,13 +1123,16 @@
       <c r="D26" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" s="8" customFormat="1">
+      <c r="E26" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="8" customFormat="1">
       <c r="A27" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="8" customFormat="1">
+    <row r="28" spans="1:5" s="8" customFormat="1">
       <c r="A28" s="9" t="s">
         <v>4</v>
       </c>
@@ -1078,13 +1145,16 @@
       <c r="D28" s="8">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" s="4" customFormat="1">
+      <c r="E28" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="4" customFormat="1">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="4" customFormat="1">
+    <row r="30" spans="1:5" s="4" customFormat="1">
       <c r="A30" s="6" t="s">
         <v>14</v>
       </c>
@@ -1094,8 +1164,11 @@
       <c r="D30" s="4">
         <v>13977</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" s="4" customFormat="1">
+      <c r="E30" s="4">
+        <v>13977</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="4" customFormat="1">
       <c r="A31" s="6" t="s">
         <v>15</v>
       </c>
@@ -1105,8 +1178,11 @@
       <c r="D31" s="4">
         <v>986</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" s="4" customFormat="1">
+      <c r="E31" s="4">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="4" customFormat="1">
       <c r="A32" s="6" t="s">
         <v>4</v>
       </c>
@@ -1116,13 +1192,16 @@
       <c r="D32" s="4">
         <v>14963</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" s="8" customFormat="1">
+      <c r="E32" s="4">
+        <v>14963</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="8" customFormat="1">
       <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="8" customFormat="1">
+    <row r="34" spans="1:5" s="8" customFormat="1">
       <c r="A34" s="9" t="s">
         <v>4</v>
       </c>
@@ -1132,13 +1211,16 @@
       <c r="D34" s="8">
         <v>1792</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" s="4" customFormat="1">
+      <c r="E34" s="8">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="4" customFormat="1">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1151,13 +1233,16 @@
       <c r="D36" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" s="8" customFormat="1">
+      <c r="E36" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="8" customFormat="1">
       <c r="A37" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="8" customFormat="1">
+    <row r="38" spans="1:5" s="8" customFormat="1">
       <c r="A38" s="9" t="s">
         <v>4</v>
       </c>
@@ -1167,16 +1252,19 @@
       <c r="D38" s="8">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E38" s="8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:4" s="14" customFormat="1">
+    <row r="43" spans="1:5" s="14" customFormat="1">
       <c r="A43" s="14" t="s">
         <v>52</v>
       </c>
@@ -1186,8 +1274,11 @@
       <c r="D43" s="14">
         <v>-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" s="14" customFormat="1">
+      <c r="E43" s="14">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="14" customFormat="1">
       <c r="A44" s="14" t="s">
         <v>53</v>
       </c>
@@ -1197,8 +1288,11 @@
       <c r="D44" s="14">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" s="14" customFormat="1">
+      <c r="E44" s="14">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="14" customFormat="1">
       <c r="A45" s="14" t="s">
         <v>54</v>
       </c>
@@ -1208,13 +1302,16 @@
       <c r="D45" s="14">
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" s="11" customFormat="1">
+      <c r="E45" s="14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="11" customFormat="1">
       <c r="A47" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="11" customFormat="1">
+    <row r="48" spans="1:5" s="11" customFormat="1">
       <c r="A48" s="11" t="s">
         <v>16</v>
       </c>
@@ -1227,8 +1324,11 @@
       <c r="D48" s="11">
         <v>55490</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" s="11" customFormat="1">
+      <c r="E48" s="11">
+        <v>55495</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="11" customFormat="1">
       <c r="A49" s="11" t="s">
         <v>17</v>
       </c>
@@ -1238,8 +1338,11 @@
       <c r="D49" s="11">
         <v>1388</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" s="11" customFormat="1">
+      <c r="E49" s="11">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="11" customFormat="1">
       <c r="A50" s="11" t="s">
         <v>18</v>
       </c>
@@ -1249,8 +1352,11 @@
       <c r="D50" s="11">
         <v>1079</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" s="11" customFormat="1">
+      <c r="E50" s="11">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="11" customFormat="1">
       <c r="A51" s="11" t="s">
         <v>19</v>
       </c>
@@ -1263,8 +1369,11 @@
       <c r="D51" s="11">
         <v>47</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" s="11" customFormat="1">
+      <c r="E51" s="11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="11" customFormat="1">
       <c r="A52" s="11" t="s">
         <v>20</v>
       </c>
@@ -1277,8 +1386,11 @@
       <c r="D52" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" s="11" customFormat="1">
+      <c r="E52" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="11" customFormat="1">
       <c r="A53" s="11" t="s">
         <v>4</v>
       </c>
@@ -1288,13 +1400,16 @@
       <c r="D53" s="11">
         <v>58008</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" s="13" customFormat="1">
+      <c r="E53" s="11">
+        <v>58014</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="13" customFormat="1">
       <c r="A54" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="13" customFormat="1">
+    <row r="55" spans="1:5" s="13" customFormat="1">
       <c r="A55" s="13" t="s">
         <v>21</v>
       </c>
@@ -1307,8 +1422,11 @@
       <c r="D55" s="13">
         <v>4506</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" s="13" customFormat="1">
+      <c r="E55" s="13">
+        <v>4508</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="13" customFormat="1">
       <c r="A56" s="13" t="s">
         <v>22</v>
       </c>
@@ -1318,8 +1436,11 @@
       <c r="D56" s="13">
         <v>206</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" s="13" customFormat="1">
+      <c r="E56" s="13">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="13" customFormat="1">
       <c r="A57" s="13" t="s">
         <v>4</v>
       </c>
@@ -1329,13 +1450,16 @@
       <c r="D57" s="13">
         <v>4712</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" s="11" customFormat="1">
+      <c r="E57" s="13">
+        <v>4714</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="11" customFormat="1">
       <c r="A58" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="11" customFormat="1">
+    <row r="59" spans="1:5" s="11" customFormat="1">
       <c r="A59" s="11" t="s">
         <v>23</v>
       </c>
@@ -1345,8 +1469,11 @@
       <c r="D59" s="11">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" s="11" customFormat="1">
+      <c r="E59" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="11" customFormat="1">
       <c r="A60" s="11" t="s">
         <v>24</v>
       </c>
@@ -1356,8 +1483,11 @@
       <c r="D60" s="11">
         <v>14</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" s="11" customFormat="1">
+      <c r="E60" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="11" customFormat="1">
       <c r="A61" s="11" t="s">
         <v>4</v>
       </c>
@@ -1370,13 +1500,16 @@
       <c r="D61" s="11">
         <v>26</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" s="13" customFormat="1">
+      <c r="E61" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="13" customFormat="1">
       <c r="A62" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="13" customFormat="1">
+    <row r="63" spans="1:5" s="13" customFormat="1">
       <c r="A63" s="13" t="s">
         <v>4</v>
       </c>
@@ -1389,13 +1522,16 @@
       <c r="D63" s="13">
         <v>131</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" s="11" customFormat="1">
+      <c r="E63" s="13">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="11" customFormat="1">
       <c r="A64" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="11" customFormat="1">
+    <row r="65" spans="1:5" s="11" customFormat="1">
       <c r="A65" s="11" t="s">
         <v>25</v>
       </c>
@@ -1408,8 +1544,11 @@
       <c r="D65" s="11">
         <v>16676</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" s="11" customFormat="1">
+      <c r="E65" s="11">
+        <v>16677</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="11" customFormat="1">
       <c r="A66" s="11" t="s">
         <v>26</v>
       </c>
@@ -1419,8 +1558,11 @@
       <c r="D66" s="11">
         <v>1306</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" s="11" customFormat="1">
+      <c r="E66" s="11">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="11" customFormat="1">
       <c r="A67" s="11" t="s">
         <v>4</v>
       </c>
@@ -1430,13 +1572,16 @@
       <c r="D67" s="11">
         <v>17982</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" s="13" customFormat="1">
+      <c r="E67" s="11">
+        <v>17983</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="13" customFormat="1">
       <c r="A68" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="13" customFormat="1">
+    <row r="69" spans="1:5" s="13" customFormat="1">
       <c r="A69" s="13" t="s">
         <v>4</v>
       </c>
@@ -1446,13 +1591,16 @@
       <c r="D69" s="13">
         <v>1664</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" s="11" customFormat="1">
+      <c r="E69" s="13">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="11" customFormat="1">
       <c r="A70" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="11" customFormat="1">
+    <row r="71" spans="1:5" s="11" customFormat="1">
       <c r="A71" s="11" t="s">
         <v>4</v>
       </c>
@@ -1462,13 +1610,16 @@
       <c r="D71" s="11">
         <v>19</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" s="13" customFormat="1">
+      <c r="E71" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="13" customFormat="1">
       <c r="A72" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="13" customFormat="1">
+    <row r="73" spans="1:5" s="13" customFormat="1">
       <c r="A73" s="13" t="s">
         <v>4</v>
       </c>
@@ -1477,6 +1628,9 @@
       </c>
       <c r="D73" s="13">
         <v>386</v>
+      </c>
+      <c r="E73" s="13">
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
genotyping validation update relating to the paper.
</commit_message>
<xml_diff>
--- a/tabular/genotypingAnalysis.xlsx
+++ b/tabular/genotypingAnalysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="14480" windowWidth="44000" windowHeight="11640" tabRatio="500"/>
+    <workbookView xWindow="27740" yWindow="0" windowWidth="23460" windowHeight="26720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,9 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Neither metadata, EPA nor ViPR define genotype</t>
   </si>
@@ -206,13 +209,44 @@
   </si>
   <si>
     <t>Updated clade definitions</t>
+  </si>
+  <si>
+    <t>Proportion where all methods define the same genotype</t>
+  </si>
+  <si>
+    <t>Proportion where all methods define the same subtype</t>
+  </si>
+  <si>
+    <t>Proportion where metadata defines a genotype</t>
+  </si>
+  <si>
+    <t>Proportion where HCV-GLUE defines a genotype</t>
+  </si>
+  <si>
+    <t>Proportion where ViPR defines a genotype</t>
+  </si>
+  <si>
+    <t>Proportion where metadata defines a subtype</t>
+  </si>
+  <si>
+    <t>Proportion where HCV-GLUE defines a subtype</t>
+  </si>
+  <si>
+    <t>Proportion where ViPR defines a subtype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -320,102 +354,110 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="80">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -453,6 +495,8 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -490,10 +534,18 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="75" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -825,18 +877,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="50.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="12.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="19" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -866,6 +920,9 @@
       <c r="E3" s="2">
         <v>82928</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
@@ -880,11 +937,16 @@
       <c r="E4" s="2">
         <v>1779</v>
       </c>
+      <c r="G4" s="16">
+        <f>E13/E3</f>
+        <v>0.72911441250241171</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1"/>
@@ -902,6 +964,9 @@
       <c r="E8" s="14">
         <v>-3</v>
       </c>
+      <c r="G8" s="14" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:15" s="14" customFormat="1">
       <c r="A9" s="14" t="s">
@@ -916,6 +981,10 @@
       <c r="E9" s="14">
         <v>0.4</v>
       </c>
+      <c r="G9" s="16">
+        <f>(E18+E22+E26+E28)/E3</f>
+        <v>0.79753521126760563</v>
+      </c>
     </row>
     <row r="10" spans="1:15" s="14" customFormat="1">
       <c r="A10" s="14" t="s">
@@ -930,11 +999,23 @@
       <c r="E10" s="14">
         <v>80</v>
       </c>
+      <c r="G10" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="G11" s="17">
+        <f>(E18+E22+E32+E34)/E3</f>
+        <v>0.99911971830985913</v>
+      </c>
     </row>
     <row r="12" spans="1:15" s="4" customFormat="1">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="G12" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:15" s="4" customFormat="1">
@@ -950,6 +1031,10 @@
       <c r="E13" s="4">
         <v>60464</v>
       </c>
+      <c r="G13" s="18">
+        <f>(E18+E26+E32+E36)/E3</f>
+        <v>0.91687970287478293</v>
+      </c>
       <c r="O13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1196,12 +1281,12 @@
         <v>14963</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="8" customFormat="1">
+    <row r="33" spans="1:7" s="8" customFormat="1">
       <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="8" customFormat="1">
+    <row r="34" spans="1:7" s="8" customFormat="1">
       <c r="A34" s="9" t="s">
         <v>4</v>
       </c>
@@ -1215,12 +1300,12 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1">
+    <row r="35" spans="1:7" s="4" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1">
+    <row r="36" spans="1:7" s="4" customFormat="1">
       <c r="A36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1237,12 +1322,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="8" customFormat="1">
+    <row r="37" spans="1:7" s="8" customFormat="1">
       <c r="A37" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="8" customFormat="1">
+    <row r="38" spans="1:7" s="8" customFormat="1">
       <c r="A38" s="9" t="s">
         <v>4</v>
       </c>
@@ -1255,16 +1340,26 @@
       <c r="E38" s="8">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="G38" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="G39" s="16">
+        <f>E48/E3</f>
+        <v>0.66919496430638625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="G41" s="16"/>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:5" s="14" customFormat="1">
+    <row r="43" spans="1:7" s="14" customFormat="1">
       <c r="A43" s="14" t="s">
         <v>52</v>
       </c>
@@ -1277,8 +1372,11 @@
       <c r="E43" s="14">
         <v>-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" s="14" customFormat="1">
+      <c r="G43" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="14" customFormat="1">
       <c r="A44" s="14" t="s">
         <v>53</v>
       </c>
@@ -1291,8 +1389,12 @@
       <c r="E44" s="14">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" s="14" customFormat="1">
+      <c r="G44" s="16">
+        <f>(E53+E57+E61+E63)/E3</f>
+        <v>0.75821194289021798</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="14" customFormat="1">
       <c r="A45" s="14" t="s">
         <v>54</v>
       </c>
@@ -1305,13 +1407,25 @@
       <c r="E45" s="14">
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" s="11" customFormat="1">
+      <c r="G45" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="G46" s="17">
+        <f>(E53+E57+E67+E69)/E3</f>
+        <v>0.99336774069071965</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="11" customFormat="1">
       <c r="A47" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" s="11" customFormat="1">
+      <c r="G47" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="11" customFormat="1">
       <c r="A48" s="11" t="s">
         <v>16</v>
       </c>
@@ -1326,6 +1440,10 @@
       </c>
       <c r="E48" s="11">
         <v>55495</v>
+      </c>
+      <c r="G48" s="18">
+        <f>(E53+E61+E67+E71)/E3</f>
+        <v>0.91687970287478293</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="11" customFormat="1">

</xml_diff>